<commit_message>
Deploying to gh-pages from  @ 9042cc3fc643650e277c199cd96e95fb18f86d96 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-1-1.xlsx
+++ b/assets/excel/2021_1-1-1.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF52D09D-2AFA-499F-AD59-764A39F7C250}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C638A22-4C5A-4C8C-8F4A-0D29E2F7D47E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{61A8B6FB-8F47-4AE9-B753-E1770030DEA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -243,6 +240,12 @@
   </si>
   <si>
     <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>1) Im Berichtsjahr 2011 erfolgte die Umstellung auf die Ergebnisse des Zensus 2011 als neue Basis für die Bevölkerungsfortschreibung. Aufgrund der unterschiedlichen Fortschreibungsbasis ist die Vergleichbarkeit der einzelnen Jahre untereinander eingeschränkt.</t>
+  </si>
+  <si>
+    <t>Quelle: Bevölkerungsfortschreibung</t>
   </si>
 </sst>
 </file>
@@ -507,120 +510,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="1_1_1_Download"/>
-      <sheetName val="A1_2020_Berechnung"/>
-      <sheetName val="A1_2020_bearbeitet"/>
-      <sheetName val="A1_2020_Rohdaten"/>
-      <sheetName val="CSV_Vorbereitung_Anzahl"/>
-      <sheetName val="CSV_Vorbereitung_Veränderung"/>
-      <sheetName val="CSV_Vorbereitung_alt"/>
-      <sheetName val="Veränderung"/>
-      <sheetName val="A1_2019"/>
-      <sheetName val="2019_A1_Karte"/>
-      <sheetName val="A1_Berechnung"/>
-      <sheetName val="Roh_Göttingen"/>
-      <sheetName val="A1_2019_roh"/>
-      <sheetName val="A1_2018_roh"/>
-      <sheetName val="A1_2017"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="10">
-          <cell r="B10">
-            <v>1</v>
-          </cell>
-          <cell r="C10">
-            <v>2</v>
-          </cell>
-          <cell r="D10">
-            <v>3</v>
-          </cell>
-          <cell r="E10">
-            <v>4</v>
-          </cell>
-          <cell r="F10">
-            <v>5</v>
-          </cell>
-          <cell r="G10">
-            <v>6</v>
-          </cell>
-          <cell r="H10">
-            <v>7</v>
-          </cell>
-          <cell r="I10">
-            <v>8</v>
-          </cell>
-          <cell r="J10">
-            <v>9</v>
-          </cell>
-          <cell r="K10">
-            <v>10</v>
-          </cell>
-          <cell r="L10">
-            <v>11</v>
-          </cell>
-          <cell r="M10">
-            <v>12</v>
-          </cell>
-          <cell r="N10">
-            <v>13</v>
-          </cell>
-          <cell r="O10">
-            <v>14</v>
-          </cell>
-          <cell r="P10">
-            <v>15</v>
-          </cell>
-          <cell r="Q10">
-            <v>16</v>
-          </cell>
-          <cell r="R10">
-            <v>17</v>
-          </cell>
-          <cell r="S10">
-            <v>18</v>
-          </cell>
-          <cell r="T10">
-            <v>19</v>
-          </cell>
-          <cell r="U10">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="B64" t="str">
-            <v>1) Im Berichtsjahr 2011 erfolgte die Umstellung auf die Ergebnisse des Zensus 2011 als neue Basis für die Bevölkerungsfortschreibung. Aufgrund der unterschiedlichen Fortschreibungsbasis ist die Vergleichbarkeit der einzelnen Jahre untereinander eingeschränkt.</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="B67" t="str">
-            <v>Quelle: Bevölkerungsfortschreibung</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -923,8 +812,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:U70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,83 +960,63 @@
     </row>
     <row r="10" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
-        <f>[1]A1_2020_Berechnung!B10</f>
         <v>1</v>
       </c>
       <c r="C10" s="4">
-        <f>[1]A1_2020_Berechnung!C10</f>
         <v>2</v>
       </c>
       <c r="D10" s="4">
-        <f>[1]A1_2020_Berechnung!D10</f>
         <v>3</v>
       </c>
       <c r="E10" s="4">
-        <f>[1]A1_2020_Berechnung!E10</f>
         <v>4</v>
       </c>
       <c r="F10" s="4">
-        <f>[1]A1_2020_Berechnung!F10</f>
         <v>5</v>
       </c>
       <c r="G10" s="4">
-        <f>[1]A1_2020_Berechnung!G10</f>
         <v>6</v>
       </c>
       <c r="H10" s="4">
-        <f>[1]A1_2020_Berechnung!H10</f>
         <v>7</v>
       </c>
       <c r="I10" s="4">
-        <f>[1]A1_2020_Berechnung!I10</f>
         <v>8</v>
       </c>
       <c r="J10" s="4">
-        <f>[1]A1_2020_Berechnung!J10</f>
         <v>9</v>
       </c>
       <c r="K10" s="4">
-        <f>[1]A1_2020_Berechnung!K10</f>
         <v>10</v>
       </c>
       <c r="L10" s="4">
-        <f>[1]A1_2020_Berechnung!L10</f>
         <v>11</v>
       </c>
       <c r="M10" s="4">
-        <f>[1]A1_2020_Berechnung!M10</f>
         <v>12</v>
       </c>
       <c r="N10" s="4">
-        <f>[1]A1_2020_Berechnung!N10</f>
         <v>13</v>
       </c>
       <c r="O10" s="4">
-        <f>[1]A1_2020_Berechnung!O10</f>
         <v>14</v>
       </c>
       <c r="P10" s="4">
-        <f>[1]A1_2020_Berechnung!P10</f>
         <v>15</v>
       </c>
       <c r="Q10" s="4">
-        <f>[1]A1_2020_Berechnung!Q10</f>
         <v>16</v>
       </c>
       <c r="R10" s="4">
-        <f>[1]A1_2020_Berechnung!R10</f>
         <v>17</v>
       </c>
       <c r="S10" s="4">
-        <f>[1]A1_2020_Berechnung!S10</f>
         <v>18</v>
       </c>
       <c r="T10" s="4">
-        <f>[1]A1_2020_Berechnung!T10</f>
         <v>19</v>
       </c>
       <c r="U10" s="4">
-        <f>[1]A1_2020_Berechnung!U10</f>
         <v>20</v>
       </c>
     </row>
@@ -4377,15 +4246,13 @@
     </row>
     <row r="63" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="8" t="str">
-        <f>[1]A1_2020_Berechnung!B64</f>
-        <v>1) Im Berichtsjahr 2011 erfolgte die Umstellung auf die Ergebnisse des Zensus 2011 als neue Basis für die Bevölkerungsfortschreibung. Aufgrund der unterschiedlichen Fortschreibungsbasis ist die Vergleichbarkeit der einzelnen Jahre untereinander eingeschränkt.</v>
+      <c r="B64" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="str">
-        <f>[1]A1_2020_Berechnung!B67</f>
-        <v>Quelle: Bevölkerungsfortschreibung</v>
+      <c r="B65" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 49040ec61a4cdbe2e54d3b9cdb0de07abe0c763e 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-1-1.xlsx
+++ b/assets/excel/2021_1-1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C638A22-4C5A-4C8C-8F4A-0D29E2F7D47E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E6D53-E56F-4A9D-99E9-CDFF68900B15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{61A8B6FB-8F47-4AE9-B753-E1770030DEA3}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangabe gestattet.</t>
   </si>
   <si>
-    <t>https://www.integrationsmonitoring-niedersachsen.de.</t>
-  </si>
-  <si>
     <t>Salzgitter  Stadt</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Quelle: Bevölkerungsfortschreibung</t>
+  </si>
+  <si>
+    <t>https://www.integrationsmonitoring.niedersachsen.de.</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
   <dimension ref="B1:U70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="11" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="15">
         <v>245273</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="12" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="15">
         <v>107726</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="13" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="15">
         <v>121199</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="14" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="15">
         <v>175298</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="15" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="15">
         <v>151452</v>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="16" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="15">
         <v>97749</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="17" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="15">
         <v>146690</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="18" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="15">
         <v>134581</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="19" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="15">
         <v>126460</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="20" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="15">
         <v>344905</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="21" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="16">
         <v>1650435</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="22" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="15">
         <v>1128543</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="23" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="15">
         <v>515729</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="24" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="15">
         <v>612814</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="25" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="15">
         <v>215548</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="26" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="15">
         <v>159840</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="27" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="15">
         <v>290643</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="28" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="15">
         <v>77918</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="29" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="15">
         <v>125870</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="30" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="15">
         <v>165557</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="31" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" s="16">
         <v>2163919</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="32" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="15">
         <v>182444</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="33" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="15">
         <v>205276</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="34" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="15">
         <v>241827</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="35" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="15">
         <v>51352</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="36" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" s="15">
         <v>175441</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="37" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="15">
         <v>112741</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="38" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="15">
         <v>164875</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="39" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="15">
         <v>142678</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="40" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" s="15">
         <v>196475</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="41" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" s="15">
         <v>96940</v>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="42" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="15">
         <v>134084</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="43" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" s="16">
         <v>1704133</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="44" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="15">
         <v>75916</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="45" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="15">
         <v>51693</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="46" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" s="15">
         <v>158565</v>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="47" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" s="15">
         <v>163814</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="48" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" s="15">
         <v>83552</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="49" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" s="15">
         <v>115891</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="50" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" s="15">
         <v>190128</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="51" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="15">
         <v>155642</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="52" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="15">
         <v>310088</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="53" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" s="15">
         <v>101412</v>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="54" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" s="15">
         <v>134442</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="55" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" s="15">
         <v>165056</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="56" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" s="15">
         <v>125731</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="57" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="15">
         <v>359449</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="58" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" s="15">
         <v>132401</v>
@@ -3998,7 +3998,7 @@
     </row>
     <row r="59" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="15">
         <v>93725</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="60" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" s="15">
         <v>57954</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="61" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="16">
         <v>2475459</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="62" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="16">
         <v>7993946</v>
@@ -4247,12 +4247,12 @@
     <row r="63" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="70" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="17" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ f7eb591a9abaf8da2b48c46bbfed4422b028fa5c 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-1-1.xlsx
+++ b/assets/excel/2021_1-1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E6D53-E56F-4A9D-99E9-CDFF68900B15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D791E03D-B128-42A9-A4F2-377798744A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{61A8B6FB-8F47-4AE9-B753-E1770030DEA3}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Göttingen</t>
   </si>
   <si>
-    <t>Stat. Region Braunschweig</t>
-  </si>
-  <si>
     <t>Hannover  Region</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Schaumburg</t>
   </si>
   <si>
-    <t>Stat. Region Hannover</t>
-  </si>
-  <si>
     <t>Celle</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>Verden</t>
   </si>
   <si>
-    <t>Stat. Region Lüneburg</t>
-  </si>
-  <si>
     <t>Delmenhorst  Stadt</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
     <t>Wittmund</t>
   </si>
   <si>
-    <t>Stat. Region Weser-Ems</t>
-  </si>
-  <si>
     <t>Niedersachsen</t>
   </si>
   <si>
@@ -246,6 +234,18 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de.</t>
+  </si>
+  <si>
+    <t>Statistische Region Braunschweig</t>
+  </si>
+  <si>
+    <t>Statistische Region Hannover</t>
+  </si>
+  <si>
+    <t>Statistische Region Lüneburg</t>
+  </si>
+  <si>
+    <t>Statistische Region Weser-Ems</t>
   </si>
 </sst>
 </file>
@@ -812,8 +812,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:U70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="21" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C21" s="16">
         <v>1650435</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="22" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="15">
         <v>1128543</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="23" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="15">
         <v>515729</v>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="24" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="15">
         <v>612814</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="25" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="15">
         <v>215548</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="26" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="15">
         <v>159840</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="27" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="15">
         <v>290643</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="28" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="15">
         <v>77918</v>
@@ -2138,7 +2138,7 @@
     </row>
     <row r="29" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="15">
         <v>125870</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="30" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="15">
         <v>165557</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="31" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C31" s="16">
         <v>2163919</v>
@@ -2324,7 +2324,7 @@
     </row>
     <row r="32" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="15">
         <v>182444</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="33" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" s="15">
         <v>205276</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="34" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="15">
         <v>241827</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="35" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="15">
         <v>51352</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="36" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" s="15">
         <v>175441</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="37" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="15">
         <v>112741</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="38" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" s="15">
         <v>164875</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="39" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="15">
         <v>142678</v>
@@ -2820,7 +2820,7 @@
     </row>
     <row r="40" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" s="15">
         <v>196475</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="41" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" s="15">
         <v>96940</v>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="42" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" s="15">
         <v>134084</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="43" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C43" s="16">
         <v>1704133</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="44" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C44" s="15">
         <v>75916</v>
@@ -3130,7 +3130,7 @@
     </row>
     <row r="45" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C45" s="15">
         <v>51693</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="46" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C46" s="15">
         <v>158565</v>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="47" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C47" s="15">
         <v>163814</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="48" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C48" s="15">
         <v>83552</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="49" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C49" s="15">
         <v>115891</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="50" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C50" s="15">
         <v>190128</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="51" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C51" s="15">
         <v>155642</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="52" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C52" s="15">
         <v>310088</v>
@@ -3626,7 +3626,7 @@
     </row>
     <row r="53" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C53" s="15">
         <v>101412</v>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="54" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C54" s="15">
         <v>134442</v>
@@ -3750,7 +3750,7 @@
     </row>
     <row r="55" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C55" s="15">
         <v>165056</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="56" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C56" s="15">
         <v>125731</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="57" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C57" s="15">
         <v>359449</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="58" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C58" s="15">
         <v>132401</v>
@@ -3998,7 +3998,7 @@
     </row>
     <row r="59" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C59" s="15">
         <v>93725</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="60" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C60" s="15">
         <v>57954</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="61" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C61" s="16">
         <v>2475459</v>
@@ -4184,7 +4184,7 @@
     </row>
     <row r="62" spans="2:21" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C62" s="16">
         <v>7993946</v>
@@ -4247,12 +4247,12 @@
     <row r="63" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="2:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="70" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>